<commit_message>
Update Training Backend Springboot - Aldi lukito.xlsx
</commit_message>
<xml_diff>
--- a/member/aldi/Training Backend Springboot - Aldi lukito.xlsx
+++ b/member/aldi/Training Backend Springboot - Aldi lukito.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Deni Setiawan\Desktop\training-springboot-aldi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Deni Setiawan\Data\github\software-engineer-upgrade\.github\member\aldi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F9B877F-81A9-4DF7-80B9-44795926CFBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E853DA91-946E-4506-A5E3-F10656777CDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -58,9 +58,6 @@
   </si>
   <si>
     <t>github</t>
-  </si>
-  <si>
-    <t>audience</t>
   </si>
   <si>
     <t>reference</t>
@@ -92,9 +89,6 @@
     <t>organization</t>
   </si>
   <si>
-    <t>https://github.com/training-backend-springboot</t>
-  </si>
-  <si>
     <t xml:space="preserve">- Installation Docker in windows 11 
 - getting started with Docker
 - getting started with docker-compose &amp; docker-compose.yml
@@ -110,6 +104,12 @@
   </si>
   <si>
     <t>NexSOFT office</t>
+  </si>
+  <si>
+    <t>https://github.com/software-engineer-upgrade</t>
+  </si>
+  <si>
+    <t>url repo</t>
   </si>
 </sst>
 </file>
@@ -229,34 +229,34 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -542,8 +542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B5:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -562,235 +562,236 @@
   </cols>
   <sheetData>
     <row r="5" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" s="3" t="s">
+      <c r="E5" s="14"/>
+      <c r="F5" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="I5" s="14" t="s">
         <v>8</v>
       </c>
       <c r="J5" s="4" t="s">
         <v>10</v>
       </c>
       <c r="K5" s="4"/>
-      <c r="L5" s="5" t="s">
+      <c r="L5" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="13"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L6" s="11"/>
+    </row>
+    <row r="7" spans="2:12" ht="156.75" x14ac:dyDescent="0.45">
+      <c r="B7" s="8">
+        <v>1</v>
+      </c>
+      <c r="C7" s="10">
+        <v>45050</v>
+      </c>
+      <c r="D7" s="9">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E7" s="9">
+        <v>0.75</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I7" s="6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="F6" s="12"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K6" s="6" t="s">
+      <c r="J7" s="5"/>
+      <c r="K7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="L6" s="5"/>
-    </row>
-    <row r="7" spans="2:12" ht="156.75" x14ac:dyDescent="0.45">
-      <c r="B7" s="10">
-        <v>1</v>
-      </c>
-      <c r="C7" s="14">
-        <v>45050</v>
-      </c>
-      <c r="D7" s="13">
-        <v>0.70833333333333337</v>
-      </c>
-      <c r="E7" s="13">
-        <v>0.75</v>
-      </c>
-      <c r="F7" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="H7" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="I7" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="J7" s="7"/>
-      <c r="K7" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="L7" s="9" t="s">
-        <v>15</v>
+      <c r="L7" s="7" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B8" s="10"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B9" s="10"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B10" s="10"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B11" s="10"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B12" s="10"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="7"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B13" s="10"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B14" s="10"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="7"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B15" s="10"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="7"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B16" s="10"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B17" s="10"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="7"/>
-      <c r="L17" s="7"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B18" s="10"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="7"/>
-      <c r="L18" s="7"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="B5:B6"/>
     <mergeCell ref="L5:L6"/>
     <mergeCell ref="F5:F6"/>
     <mergeCell ref="D5:E5"/>
@@ -798,7 +799,6 @@
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="H5:H6"/>
     <mergeCell ref="I5:I6"/>
-    <mergeCell ref="B5:B6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="L7" r:id="rId1" xr:uid="{4B3BDFC1-BDF3-4F78-B679-DE31F972E2C1}"/>

</xml_diff>